<commit_message>
Beta Heat Map and Beta Exposure modified
</commit_message>
<xml_diff>
--- a/funds/Interval/Interval_INDSH_risk_report_20240221.xlsx
+++ b/funds/Interval/Interval_INDSH_risk_report_20240221.xlsx
@@ -23,7 +23,7 @@
     <sheet name="FactorCorrels" sheetId="14" r:id="rId14"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">BetaExposures!$A$1:$S$251</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">BetaExposures!$A$1:$V$251</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Dashboard!$A$1:$R$251</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="7">ExpReport!$A$1:$O$251</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="13">FactorCorrels!$A$1:$C$251</definedName>
@@ -4675,13 +4675,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
@@ -4705,16 +4705,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6094,7 +6094,7 @@
 <file path=xl/tables/table177.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="177" name="options_delta" displayName="options_delta" ref="B5:J20" totalsRowShown="0">
   <tableColumns count="9">
-    <tableColumn id="1" name="Position"/>
+    <tableColumn id="1" name="Position" dataDxfId="1"/>
     <tableColumn id="2" name="Cost" dataDxfId="1"/>
     <tableColumn id="3" name="MV" dataDxfId="1"/>
     <tableColumn id="4" name="P&amp;L" dataDxfId="1"/>
@@ -12002,7 +12002,7 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="16" customHeight="1">
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>457</v>
       </c>
       <c r="C6" s="6">
@@ -12031,7 +12031,7 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="16" customHeight="1">
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>458</v>
       </c>
       <c r="C7" s="6">
@@ -12060,7 +12060,7 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="16" customHeight="1">
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>459</v>
       </c>
       <c r="C8" s="6">
@@ -12089,7 +12089,7 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="16" customHeight="1">
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>460</v>
       </c>
       <c r="C9" s="6">
@@ -12118,7 +12118,7 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="16" customHeight="1">
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>461</v>
       </c>
       <c r="C10" s="6">
@@ -12147,7 +12147,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="16" customHeight="1">
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>462</v>
       </c>
       <c r="C11" s="6">
@@ -12176,7 +12176,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="16" customHeight="1">
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>463</v>
       </c>
       <c r="C12" s="6">
@@ -12205,7 +12205,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="16" customHeight="1">
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>464</v>
       </c>
       <c r="C13" s="6">
@@ -12234,7 +12234,7 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="16" customHeight="1">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>465</v>
       </c>
       <c r="C14" s="6">
@@ -12263,7 +12263,7 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="16" customHeight="1">
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>466</v>
       </c>
       <c r="C15" s="6">
@@ -12292,7 +12292,7 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="16" customHeight="1">
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>467</v>
       </c>
       <c r="C16" s="6">
@@ -12321,7 +12321,7 @@
       </c>
     </row>
     <row r="17" spans="2:10" ht="16" customHeight="1">
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>468</v>
       </c>
       <c r="C17" s="6">
@@ -12350,7 +12350,7 @@
       </c>
     </row>
     <row r="18" spans="2:10" ht="16" customHeight="1">
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>469</v>
       </c>
       <c r="C18" s="6">
@@ -12379,7 +12379,7 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="16" customHeight="1">
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>470</v>
       </c>
       <c r="C19" s="6">
@@ -12408,7 +12408,7 @@
       </c>
     </row>
     <row r="20" spans="2:10" ht="16" customHeight="1">
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>471</v>
       </c>
       <c r="C20" s="6">
@@ -56928,19 +56928,19 @@
     <col min="1" max="1" width="8.7109375" customWidth="1"/>
     <col min="2" max="2" width="26.7109375" customWidth="1"/>
     <col min="3" max="4" width="12.7109375" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="26.7109375" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" customWidth="1"/>
-    <col min="11" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="8.7109375" customWidth="1"/>
-    <col min="14" max="14" width="26.7109375" customWidth="1"/>
-    <col min="15" max="16" width="12.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
+    <col min="5" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" customWidth="1"/>
+    <col min="8" max="9" width="12.7109375" customWidth="1"/>
+    <col min="10" max="11" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="26.7109375" customWidth="1"/>
+    <col min="13" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="26.7109375" customWidth="1"/>
+    <col min="18" max="19" width="12.7109375" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="30" customHeight="1">
+    <row r="1" spans="2:19" ht="30" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>292</v>
       </c>
@@ -56958,8 +56958,11 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="2:16" ht="16" customHeight="1">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+    </row>
+    <row r="2" spans="2:19" ht="16" customHeight="1">
       <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
@@ -56977,8 +56980,11 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
-    </row>
-    <row r="3" spans="2:16" ht="16" customHeight="1">
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" spans="2:19" ht="16" customHeight="1">
       <c r="B3" s="3">
         <v>45343</v>
       </c>
@@ -56996,8 +57002,11 @@
       <c r="N3" s="3"/>
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
-    </row>
-    <row r="5" spans="2:16" ht="16" customHeight="1">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+    </row>
+    <row r="5" spans="2:19" ht="16" customHeight="1">
       <c r="B5" s="4" t="s">
         <v>49</v>
       </c>
@@ -57011,7 +57020,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="2:16" ht="16" customHeight="1">
+    <row r="6" spans="2:19" ht="16" customHeight="1">
       <c r="B6" s="5" t="s">
         <v>53</v>
       </c>
@@ -57025,7 +57034,7 @@
         <v>0.001519961350479291</v>
       </c>
     </row>
-    <row r="7" spans="2:16" ht="16" customHeight="1">
+    <row r="7" spans="2:19" ht="16" customHeight="1">
       <c r="B7" s="5" t="s">
         <v>54</v>
       </c>
@@ -57039,7 +57048,7 @@
         <v>0.001136206529137776</v>
       </c>
     </row>
-    <row r="8" spans="2:16" ht="16" customHeight="1">
+    <row r="8" spans="2:19" ht="16" customHeight="1">
       <c r="B8" s="5" t="s">
         <v>55</v>
       </c>
@@ -57053,7 +57062,7 @@
         <v>0.0001050767899327258</v>
       </c>
     </row>
-    <row r="9" spans="2:16" ht="16" customHeight="1">
+    <row r="9" spans="2:19" ht="16" customHeight="1">
       <c r="B9" s="5" t="s">
         <v>56</v>
       </c>
@@ -57067,7 +57076,7 @@
         <v>0.001503136382488945</v>
       </c>
     </row>
-    <row r="10" spans="2:16" ht="16" customHeight="1">
+    <row r="10" spans="2:19" ht="16" customHeight="1">
       <c r="B10" s="5" t="s">
         <v>57</v>
       </c>
@@ -57081,7 +57090,7 @@
         <v>0.0008992038454785413</v>
       </c>
     </row>
-    <row r="11" spans="2:16" ht="16" customHeight="1">
+    <row r="11" spans="2:19" ht="16" customHeight="1">
       <c r="B11" s="5" t="s">
         <v>58</v>
       </c>
@@ -57095,7 +57104,7 @@
         <v>0.0004677349435997183</v>
       </c>
     </row>
-    <row r="12" spans="2:16" ht="16" customHeight="1">
+    <row r="12" spans="2:19" ht="16" customHeight="1">
       <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
@@ -57109,7 +57118,7 @@
         <v>0.0008989571140410128</v>
       </c>
     </row>
-    <row r="13" spans="2:16" ht="16" customHeight="1">
+    <row r="13" spans="2:19" ht="16" customHeight="1">
       <c r="B13" s="5" t="s">
         <v>60</v>
       </c>
@@ -57123,7 +57132,7 @@
         <v>0.001518791868236769</v>
       </c>
     </row>
-    <row r="14" spans="2:16" ht="16" customHeight="1">
+    <row r="14" spans="2:19" ht="16" customHeight="1">
       <c r="B14" s="5" t="s">
         <v>61</v>
       </c>
@@ -57137,7 +57146,7 @@
         <v>0.0009420972104787094</v>
       </c>
     </row>
-    <row r="15" spans="2:16" ht="16" customHeight="1">
+    <row r="15" spans="2:19" ht="16" customHeight="1">
       <c r="B15" s="5" t="s">
         <v>62</v>
       </c>
@@ -57151,7 +57160,7 @@
         <v>0.0007978144380508369</v>
       </c>
     </row>
-    <row r="16" spans="2:16" ht="16" customHeight="1">
+    <row r="16" spans="2:19" ht="16" customHeight="1">
       <c r="B16" s="5" t="s">
         <v>63</v>
       </c>
@@ -64163,9 +64172,9 @@
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B3:P3"/>
+    <mergeCell ref="B1:S1"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="B3:S3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup fitToHeight="0" orientation="portrait"/>

</xml_diff>